<commit_message>
Updating user_says excel agent
</commit_message>
<xml_diff>
--- a/Agent/user_says.xlsx
+++ b/Agent/user_says.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>intent</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>AnnotationParam</t>
+  </si>
+  <si>
+    <t>smartphoneName</t>
   </si>
   <si>
     <t>productCategory</t>
@@ -78,27 +81,110 @@
     <t>buy&gt;product.category</t>
   </si>
   <si>
+    <t>product.category&gt;sp.range</t>
+  </si>
+  <si>
+    <t>smartphone
+móvil
+moviles
+movil</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 comprar
 quiero hacer una compra
 estoy buscando
-quiero comprar</t>
-  </si>
-  <si>
-    <t>product.category&gt;sp.range</t>
+quiero comprar
+   Quiero hacer una compra
+  Me gustaría comprar
+  Necesito información
+  Busco información sobre productos</t>
   </si>
   <si>
     <t>quiero comprar un smartphone
 estoy buscando un móvil
 no sé que móvil comprarme
 me gustaría comprar un smartphone
-ayudame a elegir un movil</t>
-  </si>
-  <si>
-    <t>smartphone
-móvil
-moviles
-movil</t>
+ayudame a elegir un movil
+  un smartphone
+  smartphones
+  un móvil
+  quiero comprar un smartphone
+  quiero un móvil</t>
+  </si>
+  <si>
+    <t>smartphoneRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  gama baja
+  gama media
+  gama alta
+  gama premium
+quiero uno de gama baja
+quiero un móvi de media gama
+uno de rango alto
+un smartphone premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gama baja
+  gama media
+  gama alta
+  gama premium
+baja
+media
+alta
+premium
+</t>
+  </si>
+  <si>
+    <t>sp.range&gt;screen</t>
+  </si>
+  <si>
+    <t>Muéstrame el Samsung S9
+  Quiero saber más sobre el lg g6
+  Hablame sobre el sony xperia zx1 compact
+Quiero el Google Pixel 2</t>
+  </si>
+  <si>
+    <t>smartphone.selected</t>
+  </si>
+  <si>
+    <t>smartphone.selected.ecommerce</t>
+  </si>
+  <si>
+    <t>smartphoneBrand</t>
+  </si>
+  <si>
+    <t>Samsung
+LG
+lg
+sony
+Google
+Apple
+huawei</t>
+  </si>
+  <si>
+    <t>S9
+S8
+zx1 compact
+Pixel 2
+G6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  pantalla pequeña
+  pantalla mediana
+  pantalla grande</t>
+  </si>
+  <si>
+    <t>smartphoneScreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  pantalla pequeña
+  pantalla mediana
+  pantalla grande
+pequeña
+mediana
+grande</t>
   </si>
 </sst>
 </file>
@@ -582,13 +668,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -605,8 +688,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -932,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,172 +1037,211 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing cache errors with images
</commit_message>
<xml_diff>
--- a/Agent/user_says.xlsx
+++ b/Agent/user_says.xlsx
@@ -195,11 +195,6 @@
     <t>sp.selected.differences</t>
   </si>
   <si>
-    <t>Estas son las principales diferencias
-Las características en als que se diferencian son las siguientes
-Se distinguen en lo siguiente</t>
-  </si>
-  <si>
     <t>cuál es el mejor móvil calidad precio
 cuales son los mejores móviles calidad precio?
 qué móvil me recomiendas por caldiad-precio?</t>
@@ -265,6 +260,11 @@
   <si>
     <t>Estas son las valoraciones medias que me han ofrecido los usuarios
 Así han valorado el smartphone los usuarios</t>
+  </si>
+  <si>
+    <t>Estas son las principales diferencias
+Las características en las que se diferencian son las siguientes
+Se distinguen en lo siguiente</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1122,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19:F20"/>
+      <selection activeCell="F17" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,13 +1229,13 @@
         <v>37</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2"/>
     </row>
@@ -1246,7 +1246,7 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2"/>
     </row>
@@ -1341,16 +1341,16 @@
         <v>38</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -1360,21 +1360,21 @@
         <v>4</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="F19" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,24 +1386,24 @@
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added intents for ecomemrce selected
</commit_message>
<xml_diff>
--- a/Agent/user_says.xlsx
+++ b/Agent/user_says.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
   <si>
     <t>UserSays</t>
   </si>
@@ -352,12 +352,6 @@
 quiero un smartphone con carga rápida</t>
   </si>
   <si>
-    <t>Aquí lo tienes:
-Este es:
-El móvil que buscas:
-Listo!</t>
-  </si>
-  <si>
     <t>Puedes comprarlo aquí
 Estas son las tiendas donde puedes comprarlo
 Aquí tienes las tiendas online donde lo ofrecen</t>
@@ -369,9 +363,6 @@
   </si>
   <si>
     <t>La carga rápdia por ahora solo suele venir en móviles de gama alta o premium. Aquí los tienes.</t>
-  </si>
-  <si>
-    <t>sp.selected.ecommerce.selected</t>
   </si>
   <si>
     <t>Amazon
@@ -384,6 +375,28 @@
   </si>
   <si>
     <t>Aquí tienes los detalles del sitio de compra elegido</t>
+  </si>
+  <si>
+    <t>ecommerce.selected.priceTracker</t>
+  </si>
+  <si>
+    <t>ecommerce.selected</t>
+  </si>
+  <si>
+    <t>Historial de precios
+gráfica de precios
+ver los últimos precios
+ver el historial de precios</t>
+  </si>
+  <si>
+    <t>Éste es el historial de precios de los últimos días {icon1}. Puedes ahorrarte un dinerillo {icon2} si no te importa esperar ¿Quieres que te avise cuando baje de precio?
+Aquí tienes las últimas variaciones de precio {icon1}. Si quieres ahorrarte un dinerillo {icon2} puedo avisarte cuando baje de precio</t>
+  </si>
+  <si>
+    <t>Aquí lo tienes:
+Éste es:
+El móvil que buscas:
+Listo!</t>
   </si>
 </sst>
 </file>
@@ -867,7 +880,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -879,6 +892,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1213,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,10 +1334,10 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1331,13 +1347,13 @@
         <v>45</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="7" t="s">
-        <v>73</v>
+      <c r="F7" s="8" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1345,7 +1361,7 @@
         <v>44</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1358,14 +1374,14 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1375,13 +1391,13 @@
         <v>6</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1389,7 +1405,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -1552,14 +1568,14 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1568,22 +1584,22 @@
       <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7" t="s">
+      <c r="E24" s="7"/>
+      <c r="F24" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -1598,7 +1614,7 @@
         <v>70</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1616,34 +1632,40 @@
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="F29" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>

</xml_diff>